<commit_message>
Fix french language not working Added a grid on 2IR/4IR Square calibration to facilitate the placement of a wii bar
</commit_message>
<xml_diff>
--- a/translations/DriverInstall.xlsx
+++ b/translations/DriverInstall.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -31,97 +31,130 @@
     <t xml:space="preserve">.es-ES</t>
   </si>
   <si>
+    <t xml:space="preserve">.fr-FR</t>
+  </si>
+  <si>
     <t xml:space="preserve">.en-US</t>
   </si>
   <si>
+    <t xml:space="preserve">UninstallButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desinstalar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Désinstaller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uninstall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RemovingCertMsg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminando Certificado de Prueba Touchmote.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suppression du certificat de test Touchmote.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removing Test Touchmote Certificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InstallButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ErrorVmultiUninstall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error durante la desinstalación del driver vmulti: {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erreur lors de la désinstallation du pilote vmulti : {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error during vmulti driver uninstallation: {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ErrorVmultiInstall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error durante la instalación del driver vmulti: {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erreur lors de l'installation du pilote vmulti : {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error during vmulti driver installation: {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ErrorDisablingDriver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error deshabilitando driver: {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erreur lors de la désactivation du pilote. {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error disabling driver. {0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DriverUninstallSuccessfull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desinstalación de driver completada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Désinstallation du pilote réussie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver uninstallation successfull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DriverInstallTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalación del Driver de Touchmote Enhanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installation du pilote amélioré Touchmote.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Touchmote Enhanced Driver Installation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DriverInstallSuccesfull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalación de driver completada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installation du pilote réussie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver installation successfull</t>
+  </si>
+  <si>
     <t xml:space="preserve">AddingCertMsg</t>
   </si>
   <si>
+    <t xml:space="preserve">Añadiendo Certificado de Prueba Touchmote a raíz de confianza.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout du certificat de test Touchmote à la racine de confiance.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adding Touchmote Test Certificate to trusted root.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Añadiendo Certificado de Prueba Touchmote a raíz de confianza.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DriverInstallSuccesfull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Driver installation successfull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalación de driver completada.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DriverInstallTitle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Touchmote Enhanced Driver Installation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalación del Driver de Touchmote Enhanced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DriverUninstallSuccessfull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Driver uninstallation successfull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desinstalación de driver completada.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ErrorDisablingDriver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error disabling driver. {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error deshabilitando driver: {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ErrorVmultiInstall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error during vmulti driver installation: {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error durante la instalación del driver vmulti: {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ErrorVmultiUninstall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error during vmulti driver uninstallation: {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error durante la desinstalación del driver vmulti: {0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InstallButton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Install</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RemovingCertMsg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Removing Test Touchmote Certificate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminando Certificado de Prueba Touchmote.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UninstallButton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uninstall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desinstalar</t>
   </si>
 </sst>
 </file>
@@ -197,12 +230,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,10 +252,18 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -345,175 +390,177 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D1"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>4</v>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>13</v>
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>16</v>
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>19</v>
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>22</v>
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>25</v>
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>28</v>
+      <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>31</v>
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D11"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>